<commit_message>
[REF]Update - add tool intelisis progress
</commit_message>
<xml_diff>
--- a/data/mensual.xlsx
+++ b/data/mensual.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\odoo-tool\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rogelio\proyecto\odoo-tool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72447FA-BB85-43AE-A6CE-96A83B8B42AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F801E99-2C15-4EFF-9CE4-7EC7BF327446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C6D3C523-3AAD-4BFA-ABC9-BEC52FFC66BA}"/>
+    <workbookView xWindow="-17595" yWindow="3645" windowWidth="17730" windowHeight="7875" xr2:uid="{C6D3C523-3AAD-4BFA-ABC9-BEC52FFC66BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -542,16 +542,16 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -565,7 +565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -574,7 +574,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -583,7 +583,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -592,7 +592,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -601,12 +601,12 @@
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -617,7 +617,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -625,7 +625,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -633,7 +633,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -644,7 +644,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -652,7 +652,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -660,7 +660,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -668,7 +668,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -676,7 +676,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -684,7 +684,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -695,12 +695,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -708,7 +708,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -716,7 +716,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -724,7 +724,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -735,7 +735,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -746,7 +746,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -757,7 +757,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -768,10 +768,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29" s="2"/>
     </row>
   </sheetData>

</xml_diff>